<commit_message>
improve heat demand check
</commit_message>
<xml_diff>
--- a/reegis_hp/de21/data/static/energybalance_states_2012_to_2014.xlsx
+++ b/reegis_hp/de21/data/static/energybalance_states_2012_to_2014.xlsx
@@ -553,7 +553,7 @@
       <xdr:col>30</xdr:col>
       <xdr:colOff>419760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -563,7 +563,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="23385960" y="6183720"/>
-          <a:ext cx="360" cy="17640"/>
+          <a:ext cx="360" cy="17280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -630,7 +630,7 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>168480</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -640,7 +640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21478680" y="6183720"/>
-          <a:ext cx="360" cy="17640"/>
+          <a:ext cx="360" cy="17280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -707,7 +707,7 @@
       <xdr:col>30</xdr:col>
       <xdr:colOff>419760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -717,83 +717,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="23385960" y="6183720"/>
-          <a:ext cx="360" cy="17640"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="27360" rIns="27360" tIns="0" bIns="18360" anchor="ctr"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="500" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>2)</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="de-DE" sz="500" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>510120</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>510480</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="28740240" y="6832800"/>
           <a:ext cx="360" cy="17280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -861,7 +784,84 @@
       <xdr:col>37</xdr:col>
       <xdr:colOff>510480</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28740240" y="6832800"/>
+          <a:ext cx="360" cy="16920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="27360" rIns="27360" tIns="0" bIns="18360" anchor="ctr"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="de-DE" sz="500" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>2)</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="de-DE" sz="500" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>510120</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>510480</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -871,7 +871,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="28740240" y="6832800"/>
-          <a:ext cx="360" cy="17280"/>
+          <a:ext cx="360" cy="16920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1168,10 +1168,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ471"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="AG18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="AM42" activeCellId="0" sqref="AM42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="AG432" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G452" activeCellId="0" sqref="G452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40736,9 +40736,7 @@
       <c r="F452" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G452" s="13" t="n">
-        <v>10529</v>
-      </c>
+      <c r="G452" s="13"/>
       <c r="H452" s="19" t="n">
         <v>65.438592</v>
       </c>
@@ -40843,9 +40841,7 @@
       <c r="F453" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G453" s="19" t="n">
-        <v>10265.839574</v>
-      </c>
+      <c r="G453" s="19"/>
       <c r="H453" s="19" t="n">
         <v>65.22168</v>
       </c>
@@ -41561,16 +41557,16 @@
       <c r="C461" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D461" s="0"/>
+      <c r="D461" s="19" t="n">
+        <v>263.160426</v>
+      </c>
       <c r="E461" s="19" t="n">
         <v>0</v>
       </c>
       <c r="F461" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="G461" s="19" t="n">
-        <v>263.160426</v>
-      </c>
+      <c r="G461" s="0"/>
       <c r="H461" s="19" t="n">
         <v>0.216912</v>
       </c>
@@ -41675,9 +41671,7 @@
       <c r="F462" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G462" s="19" t="n">
-        <v>8995</v>
-      </c>
+      <c r="G462" s="19"/>
       <c r="H462" s="19" t="n">
         <v>5.17897</v>
       </c>
@@ -41782,9 +41776,7 @@
       <c r="F463" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G463" s="19" t="n">
-        <v>8736.74746</v>
-      </c>
+      <c r="G463" s="19"/>
       <c r="H463" s="19" t="n">
         <v>5.17897</v>
       </c>
@@ -42499,16 +42491,16 @@
       <c r="C471" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D471" s="0"/>
+      <c r="D471" s="19" t="n">
+        <v>258.25254</v>
+      </c>
       <c r="E471" s="19" t="n">
         <v>0</v>
       </c>
       <c r="F471" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="G471" s="19" t="n">
-        <v>258.25254</v>
-      </c>
+      <c r="G471" s="0"/>
       <c r="H471" s="19" t="n">
         <v>0</v>
       </c>

</xml_diff>